<commit_message>
Ajout du menu plus style css
</commit_message>
<xml_diff>
--- a/CodeHive/Files/users.xlsx
+++ b/CodeHive/Files/users.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>test</t>
   </si>
@@ -70,6 +70,24 @@
   </si>
   <si>
     <t>DedTzVKudfREK6Jia9B2Gg==</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>MrPlFV/OrrrDHZeiO+tz1YB6vkINsvdtc4n1hyUNjVs=</t>
+  </si>
+  <si>
+    <t>GjNm+Zhdefr7W9LtefsSDw==</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>NWH3CJSReh6JsrIXloaA+5EPvPgJyt1yt4P5kgF4AkU=</t>
+  </si>
+  <si>
+    <t>SGl5a0zLko4BN+bAmwBWOA==</t>
   </si>
 </sst>
 </file>
@@ -388,7 +406,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -456,6 +474,28 @@
         <v>14</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>